<commit_message>
changed date into proper format
</commit_message>
<xml_diff>
--- a/excels/lite/lite-Page-Post.xlsx
+++ b/excels/lite/lite-Page-Post.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16100" xWindow="2640" yWindow="2600"/>
+    <workbookView xWindow="2640" yWindow="2600" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" concurrentCalc="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -36,36 +41,23 @@
   <si>
     <t>Page Post Impressions Viral</t>
   </si>
-  <si>
-    <t>13/02/2019</t>
-  </si>
-  <si>
-    <t>14/02/2019</t>
-  </si>
-  <si>
-    <t>16/02/2019</t>
-  </si>
-  <si>
-    <t>19/02/2019</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -81,16 +73,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -378,20 +371,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="10"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -418,190 +407,195 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="1">
         <v>43506</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>3</v>
       </c>
-      <c r="C2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>3</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="1">
         <v>43507</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>3</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="1">
         <v>43508</v>
       </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="1">
         <v>43508</v>
       </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="n">
+      <c r="A6" s="1">
+        <v>43509</v>
+      </c>
+      <c r="B6">
         <v>98</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>8</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>5</v>
       </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>98</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" t="s">
+      <c r="A7" s="1">
+        <v>43510</v>
+      </c>
+      <c r="B7">
+        <v>173</v>
+      </c>
+      <c r="C7">
         <v>8</v>
       </c>
-      <c r="B7" t="n">
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>173</v>
       </c>
-      <c r="C7" t="n">
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1">
+        <v>43512</v>
+      </c>
+      <c r="B8">
+        <v>181</v>
+      </c>
+      <c r="C8">
         <v>8</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D8">
         <v>4</v>
       </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>173</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="n">
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>181</v>
       </c>
-      <c r="C8" t="n">
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1">
+        <v>43515</v>
+      </c>
+      <c r="B9">
+        <v>181</v>
+      </c>
+      <c r="C9">
         <v>8</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D9">
         <v>4</v>
       </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
         <v>181</v>
       </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="n">
-        <v>181</v>
-      </c>
-      <c r="C9" t="n">
-        <v>8</v>
-      </c>
-      <c r="D9" t="n">
-        <v>4</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>181</v>
-      </c>
-      <c r="G9" t="n">
+      <c r="G9">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>